<commit_message>
realizando testeo de uSD
</commit_message>
<xml_diff>
--- a/Documentacion/matriales.xlsx
+++ b/Documentacion/matriales.xlsx
@@ -11,7 +11,7 @@
     <sheet name="Hoja2" sheetId="2" r:id="rId2"/>
     <sheet name="Hoja3" sheetId="3" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="125725"/>
+  <calcPr calcId="124519"/>
 </workbook>
 </file>
 
@@ -539,8 +539,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:D91"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C13" sqref="C13"/>
+    <sheetView tabSelected="1" topLeftCell="A5" workbookViewId="0">
+      <selection activeCell="C27" sqref="C27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>

</xml_diff>

<commit_message>
test para para el accelerometro por SPI. las pruebas se estan haciendo en proteus. test de esccritura paso la prueba. test de lectura esta condicionado a una espera despues del envio de la direccion.
</commit_message>
<xml_diff>
--- a/Documentacion/matriales.xlsx
+++ b/Documentacion/matriales.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="66" uniqueCount="63">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="68" uniqueCount="65">
   <si>
     <t>material</t>
   </si>
@@ -205,6 +205,12 @@
   </si>
   <si>
     <t>gisroscopio</t>
+  </si>
+  <si>
+    <t>12p</t>
+  </si>
+  <si>
+    <t>0,1u</t>
   </si>
 </sst>
 </file>
@@ -537,13 +543,16 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:D91"/>
+  <dimension ref="A1:D93"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A5" workbookViewId="0">
-      <selection activeCell="C27" sqref="C27"/>
+    <sheetView tabSelected="1" topLeftCell="A45" workbookViewId="0">
+      <selection activeCell="C67" sqref="C67"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
+  <cols>
+    <col min="1" max="1" width="16.140625" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:3">
       <c r="A1" t="s">
@@ -956,7 +965,7 @@
         <v>22</v>
       </c>
       <c r="B48">
-        <v>100</v>
+        <v>104</v>
       </c>
       <c r="C48">
         <v>4</v>
@@ -969,7 +978,7 @@
     </row>
     <row r="50" spans="2:3">
       <c r="B50">
-        <v>10</v>
+        <v>103</v>
       </c>
       <c r="C50">
         <v>5</v>
@@ -977,10 +986,10 @@
     </row>
     <row r="51" spans="2:3">
       <c r="B51">
-        <v>1</v>
+        <v>102</v>
       </c>
       <c r="C51">
-        <v>2</v>
+        <v>4</v>
       </c>
     </row>
     <row r="52" spans="2:3">
@@ -996,12 +1005,12 @@
         <v>23</v>
       </c>
       <c r="C53">
-        <v>1</v>
+        <v>4</v>
       </c>
     </row>
     <row r="54" spans="2:3">
       <c r="B54" t="s">
-        <v>24</v>
+        <v>63</v>
       </c>
       <c r="C54">
         <v>1</v>
@@ -1009,31 +1018,31 @@
     </row>
     <row r="55" spans="2:3">
       <c r="B55" t="s">
+        <v>24</v>
+      </c>
+      <c r="C55">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="56" spans="2:3">
+      <c r="B56" t="s">
         <v>25</v>
       </c>
-      <c r="C55">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="56" spans="2:3">
-      <c r="B56">
-        <v>23</v>
-      </c>
       <c r="C56">
-        <v>1</v>
+        <v>8</v>
       </c>
     </row>
     <row r="57" spans="2:3">
       <c r="B57">
+        <v>23</v>
+      </c>
+      <c r="C57">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="58" spans="2:3">
+      <c r="B58">
         <v>82</v>
-      </c>
-      <c r="C57">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="58" spans="2:3">
-      <c r="B58" t="s">
-        <v>26</v>
       </c>
       <c r="C58">
         <v>1</v>
@@ -1041,7 +1050,7 @@
     </row>
     <row r="59" spans="2:3">
       <c r="B59" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="C59">
         <v>1</v>
@@ -1049,7 +1058,7 @@
     </row>
     <row r="60" spans="2:3">
       <c r="B60" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="C60">
         <v>1</v>
@@ -1057,7 +1066,7 @@
     </row>
     <row r="61" spans="2:3">
       <c r="B61" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="C61">
         <v>1</v>
@@ -1065,7 +1074,7 @@
     </row>
     <row r="62" spans="2:3">
       <c r="B62" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="C62">
         <v>1</v>
@@ -1073,15 +1082,15 @@
     </row>
     <row r="63" spans="2:3">
       <c r="B63" t="s">
-        <v>31</v>
+        <v>64</v>
       </c>
       <c r="C63">
-        <v>1</v>
+        <v>3</v>
       </c>
     </row>
     <row r="64" spans="2:3">
       <c r="B64" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="C64">
         <v>1</v>
@@ -1089,7 +1098,7 @@
     </row>
     <row r="65" spans="1:3">
       <c r="B65" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="C65">
         <v>1</v>
@@ -1097,34 +1106,34 @@
     </row>
     <row r="66" spans="1:3">
       <c r="B66" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="C66">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="67" spans="1:3">
-      <c r="A67" t="s">
-        <v>35</v>
-      </c>
       <c r="B67" t="s">
-        <v>36</v>
+        <v>33</v>
       </c>
       <c r="C67">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="68" spans="1:3">
       <c r="B68" t="s">
-        <v>37</v>
+        <v>34</v>
       </c>
       <c r="C68">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="69" spans="1:3">
+      <c r="A69" t="s">
+        <v>35</v>
+      </c>
       <c r="B69" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="C69">
         <v>2</v>
@@ -1132,61 +1141,58 @@
     </row>
     <row r="70" spans="1:3">
       <c r="B70" t="s">
+        <v>37</v>
+      </c>
+      <c r="C70">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="71" spans="1:3">
+      <c r="B71" t="s">
+        <v>38</v>
+      </c>
+      <c r="C71">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="72" spans="1:3">
+      <c r="B72" t="s">
         <v>39</v>
       </c>
-      <c r="C70">
+      <c r="C72">
         <v>5</v>
-      </c>
-    </row>
-    <row r="71" spans="1:3">
-      <c r="A71" t="s">
-        <v>40</v>
-      </c>
-      <c r="C71">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="72" spans="1:3">
-      <c r="A72" t="s">
-        <v>41</v>
-      </c>
-      <c r="C72">
-        <v>2</v>
       </c>
     </row>
     <row r="73" spans="1:3">
       <c r="A73" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="C73">
-        <v>7</v>
+        <v>4</v>
       </c>
     </row>
     <row r="74" spans="1:3">
       <c r="A74" t="s">
-        <v>43</v>
-      </c>
-      <c r="B74" t="s">
-        <v>44</v>
+        <v>41</v>
       </c>
       <c r="C74">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="75" spans="1:3">
-      <c r="B75" t="s">
-        <v>45</v>
+      <c r="A75" t="s">
+        <v>42</v>
       </c>
       <c r="C75">
-        <v>1</v>
+        <v>7</v>
       </c>
     </row>
     <row r="76" spans="1:3">
       <c r="A76" t="s">
-        <v>46</v>
+        <v>43</v>
       </c>
       <c r="B76" t="s">
-        <v>47</v>
+        <v>44</v>
       </c>
       <c r="C76">
         <v>1</v>
@@ -1194,82 +1200,85 @@
     </row>
     <row r="77" spans="1:3">
       <c r="B77" t="s">
+        <v>45</v>
+      </c>
+      <c r="C77">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="78" spans="1:3">
+      <c r="A78" t="s">
+        <v>46</v>
+      </c>
+      <c r="B78" t="s">
+        <v>47</v>
+      </c>
+      <c r="C78">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="79" spans="1:3">
+      <c r="B79" t="s">
         <v>48</v>
       </c>
-      <c r="C77">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="78" spans="1:3">
-      <c r="B78" s="1" t="s">
+      <c r="C79">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="80" spans="1:3">
+      <c r="B80" s="1" t="s">
         <v>49</v>
       </c>
-      <c r="C78">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="79" spans="1:3">
-      <c r="A79" t="s">
-        <v>50</v>
-      </c>
-      <c r="B79" t="s">
-        <v>51</v>
-      </c>
-      <c r="C79">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="80" spans="1:3">
-      <c r="B80" t="s">
-        <v>52</v>
-      </c>
       <c r="C80">
-        <v>3</v>
+        <v>1</v>
       </c>
     </row>
     <row r="81" spans="1:3">
       <c r="A81" t="s">
-        <v>53</v>
+        <v>50</v>
+      </c>
+      <c r="B81" t="s">
+        <v>51</v>
       </c>
       <c r="C81">
         <v>2</v>
       </c>
     </row>
     <row r="82" spans="1:3">
-      <c r="A82" t="s">
-        <v>54</v>
+      <c r="B82" t="s">
+        <v>52</v>
       </c>
       <c r="C82">
-        <v>2</v>
+        <v>3</v>
       </c>
     </row>
     <row r="83" spans="1:3">
       <c r="A83" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="C83">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="84" spans="1:3">
       <c r="A84" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="C84">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="85" spans="1:3">
       <c r="A85" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="C85">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="86" spans="1:3">
       <c r="A86" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="C86">
         <v>1</v>
@@ -1277,23 +1286,23 @@
     </row>
     <row r="87" spans="1:3">
       <c r="A87" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="C87">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="88" spans="1:3">
       <c r="A88" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="C88">
         <v>1</v>
       </c>
     </row>
     <row r="89" spans="1:3">
-      <c r="A89">
-        <v>7805</v>
+      <c r="A89" t="s">
+        <v>59</v>
       </c>
       <c r="C89">
         <v>1</v>
@@ -1301,17 +1310,33 @@
     </row>
     <row r="90" spans="1:3">
       <c r="A90" t="s">
+        <v>60</v>
+      </c>
+      <c r="C90">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="91" spans="1:3">
+      <c r="A91">
+        <v>7805</v>
+      </c>
+      <c r="C91">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="92" spans="1:3">
+      <c r="A92" t="s">
         <v>61</v>
       </c>
-      <c r="C90">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="91" spans="1:3">
-      <c r="A91" t="s">
+      <c r="C92">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="93" spans="1:3">
+      <c r="A93" t="s">
         <v>62</v>
       </c>
-      <c r="C91">
+      <c r="C93">
         <v>1</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Nueva implementacion atravez de de ADC del micro
</commit_message>
<xml_diff>
--- a/Documentacion/matriales.xlsx
+++ b/Documentacion/matriales.xlsx
@@ -217,8 +217,16 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="1">
+  <fonts count="2">
     <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
@@ -246,9 +254,10 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="3" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -543,10 +552,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:D93"/>
+  <dimension ref="A1:D94"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A45" workbookViewId="0">
-      <selection activeCell="C67" sqref="C67"/>
+      <selection activeCell="C51" sqref="C51"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
@@ -981,44 +990,44 @@
         <v>103</v>
       </c>
       <c r="C50">
-        <v>5</v>
+        <v>10</v>
       </c>
     </row>
     <row r="51" spans="2:3">
       <c r="B51">
         <v>102</v>
       </c>
-      <c r="C51">
+      <c r="C51" s="2">
         <v>4</v>
       </c>
     </row>
     <row r="52" spans="2:3">
       <c r="B52">
+        <v>333</v>
+      </c>
+      <c r="C52">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="53" spans="2:3">
+      <c r="B53">
         <v>1.5</v>
       </c>
-      <c r="C52">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="53" spans="2:3">
-      <c r="B53" t="s">
-        <v>23</v>
-      </c>
       <c r="C53">
-        <v>4</v>
+        <v>1</v>
       </c>
     </row>
     <row r="54" spans="2:3">
       <c r="B54" t="s">
-        <v>63</v>
+        <v>23</v>
       </c>
       <c r="C54">
-        <v>1</v>
+        <v>4</v>
       </c>
     </row>
     <row r="55" spans="2:3">
       <c r="B55" t="s">
-        <v>24</v>
+        <v>63</v>
       </c>
       <c r="C55">
         <v>1</v>
@@ -1026,31 +1035,31 @@
     </row>
     <row r="56" spans="2:3">
       <c r="B56" t="s">
+        <v>24</v>
+      </c>
+      <c r="C56">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="57" spans="2:3">
+      <c r="B57" t="s">
         <v>25</v>
       </c>
-      <c r="C56">
+      <c r="C57">
         <v>8</v>
-      </c>
-    </row>
-    <row r="57" spans="2:3">
-      <c r="B57">
-        <v>23</v>
-      </c>
-      <c r="C57">
-        <v>1</v>
       </c>
     </row>
     <row r="58" spans="2:3">
       <c r="B58">
+        <v>23</v>
+      </c>
+      <c r="C58">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="59" spans="2:3">
+      <c r="B59">
         <v>82</v>
-      </c>
-      <c r="C58">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="59" spans="2:3">
-      <c r="B59" t="s">
-        <v>26</v>
       </c>
       <c r="C59">
         <v>1</v>
@@ -1058,7 +1067,7 @@
     </row>
     <row r="60" spans="2:3">
       <c r="B60" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="C60">
         <v>1</v>
@@ -1066,7 +1075,7 @@
     </row>
     <row r="61" spans="2:3">
       <c r="B61" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="C61">
         <v>1</v>
@@ -1074,7 +1083,7 @@
     </row>
     <row r="62" spans="2:3">
       <c r="B62" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="C62">
         <v>1</v>
@@ -1082,23 +1091,23 @@
     </row>
     <row r="63" spans="2:3">
       <c r="B63" t="s">
-        <v>64</v>
+        <v>29</v>
       </c>
       <c r="C63">
-        <v>3</v>
+        <v>1</v>
       </c>
     </row>
     <row r="64" spans="2:3">
       <c r="B64" t="s">
-        <v>30</v>
+        <v>64</v>
       </c>
       <c r="C64">
-        <v>1</v>
+        <v>3</v>
       </c>
     </row>
     <row r="65" spans="1:3">
       <c r="B65" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="C65">
         <v>1</v>
@@ -1106,42 +1115,42 @@
     </row>
     <row r="66" spans="1:3">
       <c r="B66" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="C66">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="67" spans="1:3">
       <c r="B67" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="C67">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="68" spans="1:3">
       <c r="B68" t="s">
+        <v>33</v>
+      </c>
+      <c r="C68">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="69" spans="1:3">
+      <c r="B69" t="s">
         <v>34</v>
       </c>
-      <c r="C68">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="69" spans="1:3">
-      <c r="A69" t="s">
+      <c r="C69">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="70" spans="1:3">
+      <c r="A70" t="s">
         <v>35</v>
       </c>
-      <c r="B69" t="s">
+      <c r="B70" t="s">
         <v>36</v>
-      </c>
-      <c r="C69">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="70" spans="1:3">
-      <c r="B70" t="s">
-        <v>37</v>
       </c>
       <c r="C70">
         <v>2</v>
@@ -1149,7 +1158,7 @@
     </row>
     <row r="71" spans="1:3">
       <c r="B71" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="C71">
         <v>2</v>
@@ -1157,112 +1166,112 @@
     </row>
     <row r="72" spans="1:3">
       <c r="B72" t="s">
+        <v>38</v>
+      </c>
+      <c r="C72">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="73" spans="1:3">
+      <c r="B73" t="s">
         <v>39</v>
       </c>
-      <c r="C72">
+      <c r="C73">
         <v>5</v>
-      </c>
-    </row>
-    <row r="73" spans="1:3">
-      <c r="A73" t="s">
-        <v>40</v>
-      </c>
-      <c r="C73">
-        <v>4</v>
       </c>
     </row>
     <row r="74" spans="1:3">
       <c r="A74" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="C74">
-        <v>2</v>
+        <v>4</v>
       </c>
     </row>
     <row r="75" spans="1:3">
       <c r="A75" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="C75">
-        <v>7</v>
+        <v>2</v>
       </c>
     </row>
     <row r="76" spans="1:3">
       <c r="A76" t="s">
+        <v>42</v>
+      </c>
+      <c r="C76">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="77" spans="1:3">
+      <c r="A77" t="s">
         <v>43</v>
       </c>
-      <c r="B76" t="s">
+      <c r="B77" t="s">
         <v>44</v>
       </c>
-      <c r="C76">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="77" spans="1:3">
-      <c r="B77" t="s">
+      <c r="C77">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="78" spans="1:3">
+      <c r="B78" t="s">
         <v>45</v>
       </c>
-      <c r="C77">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="78" spans="1:3">
-      <c r="A78" t="s">
+      <c r="C78">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="79" spans="1:3">
+      <c r="A79" t="s">
         <v>46</v>
       </c>
-      <c r="B78" t="s">
+      <c r="B79" t="s">
         <v>47</v>
       </c>
-      <c r="C78">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="79" spans="1:3">
-      <c r="B79" t="s">
+      <c r="C79">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="80" spans="1:3">
+      <c r="B80" t="s">
         <v>48</v>
       </c>
-      <c r="C79">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="80" spans="1:3">
-      <c r="B80" s="1" t="s">
+      <c r="C80">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="81" spans="1:3">
+      <c r="B81" s="1" t="s">
         <v>49</v>
       </c>
-      <c r="C80">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="81" spans="1:3">
-      <c r="A81" t="s">
+      <c r="C81">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="82" spans="1:3">
+      <c r="A82" t="s">
         <v>50</v>
       </c>
-      <c r="B81" t="s">
+      <c r="B82" t="s">
         <v>51</v>
       </c>
-      <c r="C81">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="82" spans="1:3">
-      <c r="B82" t="s">
+      <c r="C82">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="83" spans="1:3">
+      <c r="B83" t="s">
         <v>52</v>
       </c>
-      <c r="C82">
+      <c r="C83">
         <v>3</v>
-      </c>
-    </row>
-    <row r="83" spans="1:3">
-      <c r="A83" t="s">
-        <v>53</v>
-      </c>
-      <c r="C83">
-        <v>2</v>
       </c>
     </row>
     <row r="84" spans="1:3">
       <c r="A84" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="C84">
         <v>2</v>
@@ -1270,15 +1279,15 @@
     </row>
     <row r="85" spans="1:3">
       <c r="A85" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="C85">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="86" spans="1:3">
       <c r="A86" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="C86">
         <v>1</v>
@@ -1286,23 +1295,23 @@
     </row>
     <row r="87" spans="1:3">
       <c r="A87" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="C87">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="88" spans="1:3">
       <c r="A88" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="C88">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="89" spans="1:3">
       <c r="A89" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="C89">
         <v>1</v>
@@ -1310,33 +1319,41 @@
     </row>
     <row r="90" spans="1:3">
       <c r="A90" t="s">
+        <v>59</v>
+      </c>
+      <c r="C90">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="91" spans="1:3">
+      <c r="A91" t="s">
         <v>60</v>
       </c>
-      <c r="C90">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="91" spans="1:3">
-      <c r="A91">
+      <c r="C91">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="92" spans="1:3">
+      <c r="A92">
         <v>7805</v>
       </c>
-      <c r="C91">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="92" spans="1:3">
-      <c r="A92" t="s">
-        <v>61</v>
-      </c>
       <c r="C92">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="93" spans="1:3">
       <c r="A93" t="s">
+        <v>61</v>
+      </c>
+      <c r="C93">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="94" spans="1:3">
+      <c r="A94" t="s">
         <v>62</v>
       </c>
-      <c r="C93">
+      <c r="C94">
         <v>1</v>
       </c>
     </row>

</xml_diff>